<commit_message>
3 new recipes, ingredients, small changes
</commit_message>
<xml_diff>
--- a/assets/data/recipes/foodProperties.xlsx
+++ b/assets/data/recipes/foodProperties.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1pab\Desktop\Pablo\showtime\assets\data\recipes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00534DA4-4D3C-4F57-B011-D26937D0B5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B16EA09-E9FF-4B0E-A638-D6D1E66D617A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
   <si>
     <t>Ingredient</t>
   </si>
@@ -325,6 +336,15 @@
   </si>
   <si>
     <t>dark chocolate</t>
+  </si>
+  <si>
+    <t>vinegar</t>
+  </si>
+  <si>
+    <t>pork ribs</t>
+  </si>
+  <si>
+    <t>cilantro</t>
   </si>
 </sst>
 </file>
@@ -688,10 +708,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC56"/>
+  <dimension ref="A1:AC59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <pane xSplit="29" ySplit="3" topLeftCell="AD4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD1" sqref="AD1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,1667 +1653,1883 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B19">
-        <v>579</v>
+        <v>26</v>
       </c>
       <c r="C19">
-        <v>38.299999999999997</v>
+        <v>0.6</v>
       </c>
       <c r="D19">
-        <v>52.4</v>
+        <v>1.9</v>
       </c>
       <c r="E19">
-        <v>36.700000000000003</v>
+        <v>1.2</v>
       </c>
       <c r="F19">
-        <v>6.12</v>
+        <v>3.1</v>
+      </c>
+      <c r="G19">
+        <v>515</v>
+      </c>
+      <c r="H19">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="I19">
+        <v>0.185</v>
       </c>
       <c r="J19">
-        <v>0.83799999999999997</v>
+        <v>0.2</v>
       </c>
       <c r="K19">
-        <v>0.3</v>
+        <v>0.54</v>
+      </c>
+      <c r="L19">
+        <v>0.08</v>
+      </c>
+      <c r="N19">
+        <v>0.126</v>
+      </c>
+      <c r="P19">
+        <v>30</v>
       </c>
       <c r="R19">
-        <v>0.59</v>
-      </c>
-      <c r="S19">
-        <v>7.2</v>
+        <v>1.7</v>
       </c>
       <c r="T19">
-        <v>567</v>
+        <v>540</v>
       </c>
       <c r="U19">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="V19">
-        <v>260</v>
+        <v>54</v>
       </c>
       <c r="W19">
-        <v>176</v>
+        <v>30</v>
       </c>
       <c r="X19">
-        <v>6.32</v>
+        <v>4.5</v>
       </c>
       <c r="Y19">
-        <v>2.65</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z19">
-        <v>1.25</v>
+        <v>0.09</v>
       </c>
       <c r="AA19">
-        <v>1.32</v>
-      </c>
-      <c r="AB19">
-        <v>8.4</v>
+        <v>0.47</v>
       </c>
       <c r="AC19">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B20">
-        <v>333</v>
+        <v>579</v>
       </c>
       <c r="C20">
-        <v>29.18</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="D20">
-        <v>2.85</v>
+        <v>52.4</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="F20">
-        <v>13.72</v>
+        <v>6.12</v>
+      </c>
+      <c r="J20">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="K20">
+        <v>0.3</v>
+      </c>
+      <c r="R20">
+        <v>0.59</v>
+      </c>
+      <c r="S20">
+        <v>7.2</v>
+      </c>
+      <c r="T20">
+        <v>567</v>
+      </c>
+      <c r="U20">
+        <v>62</v>
+      </c>
+      <c r="V20">
+        <v>260</v>
+      </c>
+      <c r="W20">
+        <v>176</v>
+      </c>
+      <c r="X20">
+        <v>6.32</v>
+      </c>
+      <c r="Y20">
+        <v>2.65</v>
+      </c>
+      <c r="Z20">
+        <v>1.25</v>
+      </c>
+      <c r="AA20">
+        <v>1.32</v>
+      </c>
+      <c r="AB20">
+        <v>8.4</v>
+      </c>
+      <c r="AC20">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B21">
-        <v>86</v>
+        <v>333</v>
       </c>
       <c r="C21">
-        <v>1.35</v>
+        <v>29.18</v>
       </c>
       <c r="D21">
-        <v>18.7</v>
+        <v>2.85</v>
       </c>
       <c r="E21">
-        <v>6.26</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>3.27</v>
+        <v>13.72</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B22">
-        <v>228</v>
+        <v>86</v>
       </c>
       <c r="C22">
-        <v>13.7</v>
+        <v>1.35</v>
       </c>
       <c r="D22">
-        <v>57.9</v>
+        <v>18.7</v>
       </c>
       <c r="E22">
-        <v>1.75</v>
+        <v>6.26</v>
       </c>
       <c r="F22">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I22">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="J22">
-        <v>2.1850000000000001</v>
-      </c>
-      <c r="N22">
-        <v>32</v>
-      </c>
-      <c r="S22">
-        <v>2.5</v>
-      </c>
-      <c r="T22">
-        <v>1525</v>
-      </c>
-      <c r="U22">
-        <v>128</v>
-      </c>
-      <c r="V22">
-        <v>734</v>
-      </c>
-      <c r="W22">
-        <v>499</v>
-      </c>
-      <c r="X22">
-        <v>13.86</v>
-      </c>
-      <c r="Y22">
-        <v>6.81</v>
-      </c>
-      <c r="Z22">
-        <v>3.7879999999999998</v>
-      </c>
-      <c r="AA22">
-        <v>3.3849999999999998</v>
-      </c>
-      <c r="AB22">
-        <v>14.3</v>
-      </c>
-      <c r="AC22">
-        <v>21</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B23">
-        <v>350</v>
+        <v>228</v>
       </c>
       <c r="C23">
-        <v>34.4</v>
+        <v>13.7</v>
       </c>
       <c r="D23">
-        <v>5.52</v>
+        <v>57.9</v>
       </c>
       <c r="E23">
-        <v>3.76</v>
+        <v>1.75</v>
       </c>
       <c r="F23">
-        <v>6.15</v>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="I23">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="J23">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="N23">
+        <v>32</v>
+      </c>
+      <c r="S23">
+        <v>2.5</v>
+      </c>
+      <c r="T23">
+        <v>1525</v>
+      </c>
+      <c r="U23">
+        <v>128</v>
+      </c>
+      <c r="V23">
+        <v>734</v>
+      </c>
+      <c r="W23">
+        <v>499</v>
+      </c>
+      <c r="X23">
+        <v>13.86</v>
+      </c>
+      <c r="Y23">
+        <v>6.81</v>
+      </c>
+      <c r="Z23">
+        <v>3.7879999999999998</v>
+      </c>
+      <c r="AA23">
+        <v>3.3849999999999998</v>
+      </c>
+      <c r="AB23">
+        <v>14.3</v>
+      </c>
+      <c r="AC23">
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>350</v>
       </c>
       <c r="C24">
-        <v>0.1</v>
+        <v>34.4</v>
       </c>
       <c r="D24">
-        <v>3.6</v>
+        <v>5.52</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>3.76</v>
       </c>
       <c r="F24">
-        <v>0.7</v>
+        <v>6.15</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B25">
-        <v>420</v>
+        <v>15</v>
       </c>
       <c r="C25">
-        <v>27.8</v>
+        <v>0.1</v>
       </c>
       <c r="D25">
-        <v>13.9</v>
+        <v>3.6</v>
       </c>
       <c r="E25">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>28.4</v>
-      </c>
-      <c r="G25">
-        <v>262</v>
-      </c>
-      <c r="H25">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="I25">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="J25">
-        <v>0.08</v>
-      </c>
-      <c r="K25">
-        <v>0.45</v>
-      </c>
-      <c r="L25">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="N25">
-        <v>6</v>
-      </c>
-      <c r="O25">
-        <v>1.4</v>
-      </c>
-      <c r="Q25">
-        <v>0.5</v>
-      </c>
-      <c r="R25">
-        <v>0.53</v>
-      </c>
-      <c r="S25">
-        <v>1.7</v>
-      </c>
-      <c r="T25">
-        <v>180</v>
-      </c>
-      <c r="U25">
-        <v>853</v>
-      </c>
-      <c r="V25">
-        <v>627</v>
-      </c>
-      <c r="W25">
-        <v>34</v>
-      </c>
-      <c r="X25">
-        <v>0.49</v>
-      </c>
-      <c r="Y25">
-        <v>4.2</v>
-      </c>
-      <c r="Z25">
-        <v>0.04</v>
-      </c>
-      <c r="AA25">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="AB25">
-        <v>34.4</v>
-      </c>
-      <c r="AC25">
-        <v>1800</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B26">
-        <v>142</v>
+        <v>420</v>
       </c>
       <c r="C26">
-        <v>9.9600000000000009</v>
+        <v>27.8</v>
       </c>
       <c r="D26">
-        <v>0.96</v>
+        <v>13.9</v>
       </c>
       <c r="E26">
-        <v>0.2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F26">
-        <v>12.4</v>
-      </c>
-      <c r="M26">
-        <v>21</v>
+        <v>28.4</v>
+      </c>
+      <c r="G26">
+        <v>262</v>
+      </c>
+      <c r="H26">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I26">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="J26">
+        <v>0.08</v>
+      </c>
+      <c r="K26">
+        <v>0.45</v>
+      </c>
+      <c r="L26">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="N26">
+        <v>6</v>
+      </c>
+      <c r="O26">
+        <v>1.4</v>
+      </c>
+      <c r="Q26">
+        <v>0.5</v>
+      </c>
+      <c r="R26">
+        <v>0.53</v>
+      </c>
+      <c r="S26">
+        <v>1.7</v>
+      </c>
+      <c r="T26">
+        <v>180</v>
+      </c>
+      <c r="U26">
+        <v>853</v>
+      </c>
+      <c r="V26">
+        <v>627</v>
+      </c>
+      <c r="W26">
+        <v>34</v>
+      </c>
+      <c r="X26">
+        <v>0.49</v>
+      </c>
+      <c r="Y26">
+        <v>4.2</v>
+      </c>
+      <c r="Z26">
+        <v>0.04</v>
+      </c>
+      <c r="AA26">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="AB26">
+        <v>34.4</v>
+      </c>
+      <c r="AC26">
+        <v>1800</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27">
-        <v>322</v>
+        <v>142</v>
       </c>
       <c r="C27">
-        <v>26.5</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="D27">
-        <v>3.59</v>
+        <v>0.96</v>
       </c>
       <c r="E27">
-        <v>0.56000000000000005</v>
+        <v>0.2</v>
       </c>
       <c r="F27">
-        <v>15.9</v>
-      </c>
-      <c r="G27">
-        <v>381</v>
-      </c>
-      <c r="H27">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="I27">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="J27">
-        <v>2.4E-2</v>
-      </c>
-      <c r="K27">
-        <v>2.99</v>
-      </c>
-      <c r="L27">
-        <v>0.35</v>
+        <v>12.4</v>
       </c>
       <c r="M27">
-        <v>27</v>
-      </c>
-      <c r="N27">
-        <v>146</v>
-      </c>
-      <c r="O27">
-        <v>1.95</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>5.4</v>
-      </c>
-      <c r="R27">
-        <v>2.58</v>
-      </c>
-      <c r="S27">
-        <v>0.7</v>
-      </c>
-      <c r="T27">
-        <v>109</v>
-      </c>
-      <c r="U27">
-        <v>129</v>
-      </c>
-      <c r="V27">
-        <v>390</v>
-      </c>
-      <c r="W27">
-        <v>5</v>
-      </c>
-      <c r="X27">
-        <v>2.73</v>
-      </c>
-      <c r="Y27">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="Z27">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="AA27">
-        <v>5.5E-2</v>
-      </c>
-      <c r="AB27">
-        <v>56</v>
-      </c>
-      <c r="AC27">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="B28">
-        <v>364</v>
+        <v>322</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>26.5</v>
       </c>
       <c r="D28">
-        <v>76.3</v>
+        <v>3.59</v>
       </c>
       <c r="E28">
-        <v>0.3</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F28">
-        <v>10</v>
+        <v>15.9</v>
+      </c>
+      <c r="G28">
+        <v>381</v>
+      </c>
+      <c r="H28">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I28">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="J28">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K28">
+        <v>2.99</v>
+      </c>
+      <c r="L28">
+        <v>0.35</v>
+      </c>
+      <c r="M28">
+        <v>27</v>
+      </c>
+      <c r="N28">
+        <v>146</v>
+      </c>
+      <c r="O28">
+        <v>1.95</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>5.4</v>
+      </c>
+      <c r="R28">
+        <v>2.58</v>
+      </c>
+      <c r="S28">
+        <v>0.7</v>
       </c>
       <c r="T28">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="U28">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="V28">
-        <v>108</v>
+        <v>390</v>
       </c>
       <c r="W28">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="X28">
-        <v>1.17</v>
+        <v>2.73</v>
       </c>
       <c r="Y28">
-        <v>0.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Z28">
-        <v>0.14399999999999999</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="AA28">
-        <v>0.68200000000000005</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AB28">
-        <v>33.9</v>
+        <v>56</v>
       </c>
       <c r="AC28">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="B29">
-        <v>143</v>
+        <v>364</v>
       </c>
       <c r="C29">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>28.2</v>
+        <v>76.3</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F29">
-        <v>6.62</v>
+        <v>10</v>
+      </c>
+      <c r="T29">
+        <v>107</v>
+      </c>
+      <c r="U29">
+        <v>15</v>
+      </c>
+      <c r="V29">
+        <v>108</v>
+      </c>
+      <c r="W29">
+        <v>22</v>
+      </c>
+      <c r="X29">
+        <v>1.17</v>
+      </c>
+      <c r="Y29">
+        <v>0.7</v>
+      </c>
+      <c r="Z29">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="AA29">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="AB29">
+        <v>33.9</v>
+      </c>
+      <c r="AC29">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30">
-        <v>357</v>
+        <v>143</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>28.2</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30">
-        <v>89</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="B31">
-        <v>379</v>
+        <v>357</v>
       </c>
       <c r="C31">
-        <v>4.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>72.8</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>3.38</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>7.95</v>
-      </c>
-      <c r="AC31">
-        <v>0.49</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32">
-        <v>35</v>
+        <v>379</v>
       </c>
       <c r="C32">
-        <v>0.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D32">
-        <v>7.9</v>
+        <v>72.8</v>
       </c>
       <c r="E32">
-        <v>3.6</v>
+        <v>3.38</v>
       </c>
       <c r="F32">
-        <v>1.9</v>
+        <v>7.95</v>
+      </c>
+      <c r="AC32">
+        <v>0.49</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B33">
-        <v>655</v>
+        <v>35</v>
       </c>
       <c r="C33">
-        <v>69.61</v>
+        <v>0.3</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="F33">
-        <v>6.38</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B34">
-        <v>340</v>
+        <v>655</v>
       </c>
       <c r="C34">
-        <v>36.1</v>
+        <v>69.61</v>
       </c>
       <c r="D34">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>2.84</v>
-      </c>
-      <c r="G34">
-        <v>411</v>
-      </c>
-      <c r="H34">
-        <v>0.02</v>
-      </c>
-      <c r="I34">
-        <v>0.188</v>
-      </c>
-      <c r="J34">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="L34">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="N34">
-        <v>4</v>
-      </c>
-      <c r="O34">
-        <v>0.16</v>
-      </c>
-      <c r="P34">
-        <v>0.6</v>
-      </c>
-      <c r="Q34">
-        <v>1.6</v>
-      </c>
-      <c r="R34">
-        <v>0.92</v>
-      </c>
-      <c r="S34">
-        <v>3.2</v>
-      </c>
-      <c r="T34">
-        <v>95</v>
-      </c>
-      <c r="U34">
-        <v>66</v>
-      </c>
-      <c r="V34">
-        <v>58</v>
-      </c>
-      <c r="W34">
-        <v>7</v>
-      </c>
-      <c r="X34">
-        <v>0.1</v>
-      </c>
-      <c r="Y34">
-        <v>0.24</v>
-      </c>
-      <c r="Z34">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="AB34">
-        <v>3</v>
-      </c>
-      <c r="AC34">
-        <v>27</v>
+        <v>6.38</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35">
-        <v>61</v>
+        <v>340</v>
       </c>
       <c r="C35">
-        <v>0.3</v>
+        <v>36.1</v>
       </c>
       <c r="D35">
-        <v>14</v>
+        <v>2.9</v>
       </c>
       <c r="E35">
-        <v>3.9</v>
+        <v>2.9</v>
       </c>
       <c r="F35">
-        <v>1.5</v>
+        <v>2.84</v>
+      </c>
+      <c r="G35">
+        <v>411</v>
+      </c>
+      <c r="H35">
+        <v>0.02</v>
+      </c>
+      <c r="I35">
+        <v>0.188</v>
+      </c>
+      <c r="J35">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L35">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N35">
+        <v>4</v>
+      </c>
+      <c r="O35">
+        <v>0.16</v>
+      </c>
+      <c r="P35">
+        <v>0.6</v>
+      </c>
+      <c r="Q35">
+        <v>1.6</v>
+      </c>
+      <c r="R35">
+        <v>0.92</v>
+      </c>
+      <c r="S35">
+        <v>3.2</v>
+      </c>
+      <c r="T35">
+        <v>95</v>
+      </c>
+      <c r="U35">
+        <v>66</v>
+      </c>
+      <c r="V35">
+        <v>58</v>
+      </c>
+      <c r="W35">
+        <v>7</v>
+      </c>
+      <c r="X35">
+        <v>0.1</v>
+      </c>
+      <c r="Y35">
+        <v>0.24</v>
+      </c>
+      <c r="Z35">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AB35">
+        <v>3</v>
+      </c>
+      <c r="AC35">
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B36">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C36">
-        <v>0.38</v>
+        <v>0.3</v>
       </c>
       <c r="D36">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36">
-        <v>13.7</v>
+        <v>3.9</v>
       </c>
       <c r="F36">
-        <v>0.82</v>
-      </c>
-      <c r="G36">
-        <v>54</v>
-      </c>
-      <c r="H36">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="I36">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="J36">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="K36">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="L36">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="N36">
-        <v>43</v>
-      </c>
-      <c r="P36">
-        <v>36.4</v>
-      </c>
-      <c r="S36">
-        <v>4.2</v>
-      </c>
-      <c r="T36">
-        <v>168</v>
-      </c>
-      <c r="U36">
-        <v>11</v>
-      </c>
-      <c r="V36">
-        <v>14</v>
-      </c>
-      <c r="W36">
-        <v>10</v>
-      </c>
-      <c r="X36">
-        <v>0.16</v>
-      </c>
-      <c r="Y36">
-        <v>0.09</v>
-      </c>
-      <c r="Z36">
-        <v>0.111</v>
-      </c>
-      <c r="AA36">
-        <v>6.3E-2</v>
-      </c>
-      <c r="AB36">
-        <v>0.6</v>
-      </c>
-      <c r="AC36">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B37">
-        <v>429</v>
+        <v>60</v>
       </c>
       <c r="C37">
-        <v>50</v>
+        <v>0.38</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>13.7</v>
       </c>
       <c r="F37">
-        <v>7.14</v>
+        <v>0.82</v>
+      </c>
+      <c r="G37">
+        <v>54</v>
+      </c>
+      <c r="H37">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I37">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J37">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="K37">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="L37">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="N37">
+        <v>43</v>
+      </c>
+      <c r="P37">
+        <v>36.4</v>
+      </c>
+      <c r="S37">
+        <v>4.2</v>
+      </c>
+      <c r="T37">
+        <v>168</v>
       </c>
       <c r="U37">
-        <v>143</v>
+        <v>11</v>
+      </c>
+      <c r="V37">
+        <v>14</v>
+      </c>
+      <c r="W37">
+        <v>10</v>
+      </c>
+      <c r="X37">
+        <v>0.16</v>
+      </c>
+      <c r="Y37">
+        <v>0.09</v>
+      </c>
+      <c r="Z37">
+        <v>0.111</v>
+      </c>
+      <c r="AA37">
+        <v>6.3E-2</v>
+      </c>
+      <c r="AB37">
+        <v>0.6</v>
       </c>
       <c r="AC37">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>61</v>
+        <v>429</v>
       </c>
       <c r="C38">
-        <v>3.2</v>
+        <v>50</v>
       </c>
       <c r="D38">
-        <v>4.9000000000000004</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>4.9000000000000004</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>3.27</v>
-      </c>
-      <c r="G38">
-        <v>32</v>
-      </c>
-      <c r="H38">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="I38">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="J38">
-        <v>0.105</v>
-      </c>
-      <c r="L38">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="M38">
-        <v>0.1</v>
-      </c>
-      <c r="O38">
-        <v>0.54</v>
-      </c>
-      <c r="R38">
-        <v>0.05</v>
-      </c>
-      <c r="S38">
-        <v>0.3</v>
-      </c>
-      <c r="T38">
-        <v>150</v>
+        <v>7.14</v>
       </c>
       <c r="U38">
-        <v>123</v>
-      </c>
-      <c r="V38">
-        <v>101</v>
-      </c>
-      <c r="W38">
-        <v>12</v>
-      </c>
-      <c r="Y38">
-        <v>0.41</v>
-      </c>
-      <c r="Z38">
-        <v>1E-3</v>
-      </c>
-      <c r="AB38">
-        <v>1.9</v>
+        <v>143</v>
       </c>
       <c r="AC38">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="B39">
-        <v>379</v>
+        <v>61</v>
       </c>
       <c r="C39">
-        <v>34.5</v>
+        <v>3.2</v>
       </c>
       <c r="D39">
-        <v>1.29</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F39">
-        <v>14.6</v>
+        <v>3.27</v>
+      </c>
+      <c r="G39">
+        <v>32</v>
+      </c>
+      <c r="H39">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I39">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="J39">
+        <v>0.105</v>
+      </c>
+      <c r="L39">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M39">
+        <v>0.1</v>
+      </c>
+      <c r="O39">
+        <v>0.54</v>
+      </c>
+      <c r="R39">
+        <v>0.05</v>
+      </c>
+      <c r="S39">
+        <v>0.3</v>
+      </c>
+      <c r="T39">
+        <v>150</v>
+      </c>
+      <c r="U39">
+        <v>123</v>
+      </c>
+      <c r="V39">
+        <v>101</v>
+      </c>
+      <c r="W39">
+        <v>12</v>
+      </c>
+      <c r="Y39">
+        <v>0.41</v>
+      </c>
+      <c r="Z39">
+        <v>1E-3</v>
+      </c>
+      <c r="AB39">
+        <v>1.9</v>
+      </c>
+      <c r="AC39">
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="B40">
-        <v>884</v>
+        <v>379</v>
       </c>
       <c r="C40">
-        <v>100</v>
+        <v>34.5</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1.29</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="R40">
-        <v>14.4</v>
-      </c>
-      <c r="S40">
-        <v>60.2</v>
-      </c>
-      <c r="T40">
-        <v>1</v>
-      </c>
-      <c r="U40">
-        <v>1</v>
-      </c>
-      <c r="X40">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="AC40">
-        <v>2</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41">
-        <v>36</v>
+        <v>884</v>
       </c>
       <c r="C41">
-        <v>0.13</v>
+        <v>100</v>
       </c>
       <c r="D41">
-        <v>7.68</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>5.76</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>0.89</v>
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>14.4</v>
+      </c>
+      <c r="S41">
+        <v>60.2</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>1</v>
+      </c>
+      <c r="X41">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AC41">
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="B42">
-        <v>393</v>
+        <v>36</v>
       </c>
       <c r="C42">
-        <v>35.71</v>
+        <v>0.13</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>7.68</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>5.76</v>
       </c>
       <c r="F42">
-        <v>17.86</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B43">
-        <v>371</v>
+        <v>393</v>
       </c>
       <c r="C43">
-        <v>1.51</v>
+        <v>35.71</v>
       </c>
       <c r="D43">
-        <v>74.67</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>13.04</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="I43">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="J43">
-        <v>5.36</v>
-      </c>
-      <c r="X43">
-        <v>3.21</v>
+        <v>17.86</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B44">
-        <v>673</v>
+        <v>371</v>
       </c>
       <c r="C44">
-        <v>68.400000000000006</v>
+        <v>1.51</v>
       </c>
       <c r="D44">
-        <v>13.1</v>
+        <v>74.67</v>
       </c>
       <c r="E44">
-        <v>3.59</v>
+        <v>2.7</v>
       </c>
       <c r="F44">
-        <v>13.7</v>
-      </c>
-      <c r="G44">
+        <v>13.04</v>
+      </c>
+      <c r="H44">
         <v>1</v>
       </c>
-      <c r="H44">
-        <v>0.36399999999999999</v>
-      </c>
       <c r="I44">
-        <v>0.22700000000000001</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="J44">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="K44">
-        <v>0.313</v>
-      </c>
-      <c r="L44">
-        <v>9.4E-2</v>
-      </c>
-      <c r="N44">
-        <v>34</v>
-      </c>
-      <c r="P44">
-        <v>0.8</v>
-      </c>
-      <c r="R44">
-        <v>9.33</v>
-      </c>
-      <c r="S44">
-        <v>53.9</v>
-      </c>
-      <c r="T44">
-        <v>597</v>
-      </c>
-      <c r="U44">
-        <v>16</v>
-      </c>
-      <c r="V44">
-        <v>575</v>
-      </c>
-      <c r="W44">
-        <v>251</v>
+        <v>5.36</v>
       </c>
       <c r="X44">
-        <v>5.53</v>
-      </c>
-      <c r="Y44">
-        <v>6.45</v>
-      </c>
-      <c r="Z44">
-        <v>1.32</v>
-      </c>
-      <c r="AA44">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="AB44">
-        <v>0.7</v>
-      </c>
-      <c r="AC44">
-        <v>2</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B45">
-        <v>263</v>
+        <v>673</v>
       </c>
       <c r="C45">
-        <v>21.2</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>3.59</v>
       </c>
       <c r="F45">
-        <v>16.899999999999999</v>
+        <v>13.7</v>
       </c>
       <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="I45">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="J45">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="K45">
+        <v>0.313</v>
+      </c>
+      <c r="L45">
+        <v>9.4E-2</v>
+      </c>
+      <c r="N45">
+        <v>34</v>
+      </c>
+      <c r="P45">
+        <v>0.8</v>
+      </c>
+      <c r="R45">
+        <v>9.33</v>
+      </c>
+      <c r="S45">
+        <v>53.9</v>
+      </c>
+      <c r="T45">
+        <v>597</v>
+      </c>
+      <c r="U45">
+        <v>16</v>
+      </c>
+      <c r="V45">
+        <v>575</v>
+      </c>
+      <c r="W45">
+        <v>251</v>
+      </c>
+      <c r="X45">
+        <v>5.53</v>
+      </c>
+      <c r="Y45">
+        <v>6.45</v>
+      </c>
+      <c r="Z45">
+        <v>1.32</v>
+      </c>
+      <c r="AA45">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AB45">
+        <v>0.7</v>
+      </c>
+      <c r="AC45">
         <v>2</v>
-      </c>
-      <c r="H45">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="I45">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="J45">
-        <v>4.34</v>
-      </c>
-      <c r="K45">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="L45">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="N45">
-        <v>5</v>
-      </c>
-      <c r="O45">
-        <v>0.7</v>
-      </c>
-      <c r="P45">
-        <v>0.7</v>
-      </c>
-      <c r="T45">
-        <v>287</v>
-      </c>
-      <c r="U45">
-        <v>14</v>
-      </c>
-      <c r="V45">
-        <v>175</v>
-      </c>
-      <c r="W45">
-        <v>19</v>
-      </c>
-      <c r="X45">
-        <v>0.88</v>
-      </c>
-      <c r="Y45">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Z45">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA45">
-        <v>0.01</v>
-      </c>
-      <c r="AB45">
-        <v>24.6</v>
-      </c>
-      <c r="AC45">
-        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B46">
-        <v>72</v>
+        <v>263</v>
       </c>
       <c r="C46">
-        <v>0.26</v>
+        <v>21.2</v>
       </c>
       <c r="D46">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>1.81</v>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="I46">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="J46">
+        <v>4.34</v>
+      </c>
+      <c r="K46">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="L46">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="N46">
+        <v>5</v>
+      </c>
+      <c r="O46">
+        <v>0.7</v>
+      </c>
+      <c r="P46">
+        <v>0.7</v>
+      </c>
+      <c r="T46">
+        <v>287</v>
+      </c>
+      <c r="U46">
+        <v>14</v>
+      </c>
+      <c r="V46">
+        <v>175</v>
+      </c>
+      <c r="W46">
+        <v>19</v>
+      </c>
+      <c r="X46">
+        <v>0.88</v>
+      </c>
+      <c r="Y46">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z46">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AA46">
+        <v>0.01</v>
+      </c>
+      <c r="AB46">
+        <v>24.6</v>
+      </c>
+      <c r="AC46">
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="B47">
-        <v>26</v>
+        <v>180</v>
       </c>
       <c r="C47">
-        <v>0.1</v>
+        <v>16</v>
       </c>
       <c r="D47">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G47">
-        <v>426</v>
+        <v>1.2</v>
       </c>
       <c r="H47">
-        <v>0.05</v>
+        <v>0.44</v>
       </c>
       <c r="I47">
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J47">
-        <v>0.6</v>
+        <v>2.6</v>
       </c>
       <c r="K47">
-        <v>0.29799999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="L47">
-        <v>6.0999999999999999E-2</v>
+        <v>0.22</v>
       </c>
       <c r="N47">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="O47">
+        <v>0.42</v>
       </c>
       <c r="P47">
-        <v>9</v>
-      </c>
-      <c r="R47">
-        <v>1.06</v>
-      </c>
-      <c r="S47">
-        <v>1.1000000000000001</v>
+        <v>0.42</v>
       </c>
       <c r="T47">
-        <v>340</v>
+        <v>172</v>
       </c>
       <c r="U47">
-        <v>21</v>
+        <v>8.4</v>
       </c>
       <c r="V47">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="W47">
-        <v>12</v>
+        <v>11.4</v>
       </c>
       <c r="X47">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="Y47">
-        <v>0.32</v>
+        <v>1.32</v>
       </c>
       <c r="Z47">
-        <v>0.127</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AA47">
-        <v>0.125</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AB47">
-        <v>0.3</v>
+        <v>14.76</v>
       </c>
       <c r="AC47">
-        <v>1</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B48">
-        <v>359</v>
+        <v>72</v>
       </c>
       <c r="C48">
-        <v>1.3</v>
+        <v>0.26</v>
       </c>
       <c r="D48">
-        <v>79.8</v>
+        <v>16</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="F48">
-        <v>6.94</v>
+        <v>1.81</v>
       </c>
       <c r="H48">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="I48">
-        <v>1.2999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J48">
-        <v>1.48</v>
-      </c>
-      <c r="K48">
-        <v>0.39</v>
+        <v>1.58</v>
       </c>
       <c r="L48">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="N48">
-        <v>97</v>
-      </c>
-      <c r="R48">
-        <v>0.04</v>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="P48">
+        <v>23.3</v>
+      </c>
+      <c r="S48">
+        <v>0.8</v>
       </c>
       <c r="T48">
-        <v>35</v>
+        <v>446</v>
       </c>
       <c r="U48">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="V48">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="W48">
-        <v>12</v>
+        <v>22.3</v>
       </c>
       <c r="X48">
-        <v>1.2</v>
+        <v>0.37</v>
       </c>
       <c r="Y48">
-        <v>0.49</v>
+        <v>0.37</v>
       </c>
       <c r="Z48">
-        <v>6.9000000000000006E-2</v>
+        <v>0.13</v>
       </c>
       <c r="AA48">
-        <v>0.47199999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="AB48">
-        <v>7.5</v>
+        <v>2</v>
       </c>
       <c r="AC48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="B49">
-        <v>270</v>
+        <v>26</v>
       </c>
       <c r="C49">
-        <v>3.6</v>
+        <v>0.1</v>
       </c>
       <c r="D49">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E49">
-        <v>5.3</v>
+        <v>2.8</v>
       </c>
       <c r="F49">
-        <v>9.4</v>
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>426</v>
       </c>
       <c r="H49">
-        <v>0.50700000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="I49">
-        <v>0.24</v>
+        <v>0.11</v>
       </c>
       <c r="J49">
-        <v>4.76</v>
+        <v>0.6</v>
       </c>
       <c r="K49">
-        <v>0.54800000000000004</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="L49">
-        <v>9.1999999999999998E-2</v>
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N49">
+        <v>16</v>
+      </c>
+      <c r="P49">
+        <v>9</v>
+      </c>
+      <c r="R49">
+        <v>1.06</v>
+      </c>
+      <c r="S49">
+        <v>1.1000000000000001</v>
       </c>
       <c r="T49">
-        <v>117</v>
+        <v>340</v>
       </c>
       <c r="U49">
-        <v>211</v>
+        <v>21</v>
       </c>
       <c r="V49">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="W49">
-        <v>26.9</v>
+        <v>12</v>
       </c>
       <c r="X49">
-        <v>3.36</v>
+        <v>0.8</v>
       </c>
       <c r="Y49">
-        <v>0.88</v>
+        <v>0.32</v>
       </c>
       <c r="Z49">
-        <v>0.124</v>
+        <v>0.127</v>
       </c>
       <c r="AA49">
-        <v>0.63200000000000001</v>
+        <v>0.125</v>
       </c>
       <c r="AB49">
-        <v>23.2</v>
+        <v>0.3</v>
       </c>
       <c r="AC49">
-        <v>400</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="D50">
-        <v>77</v>
+        <v>79.8</v>
       </c>
       <c r="E50">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>7</v>
+        <v>6.94</v>
+      </c>
+      <c r="H50">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="I50">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J50">
+        <v>1.48</v>
+      </c>
+      <c r="K50">
+        <v>0.39</v>
+      </c>
+      <c r="L50">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N50">
+        <v>97</v>
+      </c>
+      <c r="R50">
+        <v>0.04</v>
       </c>
       <c r="T50">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="U50">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="V50">
+        <v>43</v>
+      </c>
+      <c r="W50">
+        <v>12</v>
       </c>
       <c r="X50">
-        <v>1.0900000000000001</v>
+        <v>1.2</v>
+      </c>
+      <c r="Y50">
+        <v>0.49</v>
+      </c>
+      <c r="Z50">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AA50">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="AB50">
+        <v>7.5</v>
       </c>
       <c r="AC50">
-        <v>106</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B51">
-        <v>36</v>
+        <v>270</v>
       </c>
       <c r="C51">
-        <v>0.22</v>
+        <v>3.6</v>
       </c>
       <c r="D51">
-        <v>7.96</v>
+        <v>49</v>
       </c>
       <c r="E51">
-        <v>4.8600000000000003</v>
+        <v>5.3</v>
       </c>
       <c r="F51">
-        <v>0.64</v>
-      </c>
-      <c r="M51">
-        <v>3.7</v>
-      </c>
-      <c r="P51">
-        <v>59.6</v>
+        <v>9.4</v>
+      </c>
+      <c r="H51">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="I51">
+        <v>0.24</v>
+      </c>
+      <c r="J51">
+        <v>4.76</v>
+      </c>
+      <c r="K51">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="L51">
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="T51">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="U51">
-        <v>17</v>
+        <v>211</v>
       </c>
       <c r="V51">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="W51">
-        <v>12.5</v>
+        <v>26.9</v>
       </c>
       <c r="X51">
-        <v>0.26</v>
+        <v>3.36</v>
       </c>
       <c r="Y51">
-        <v>0.11</v>
+        <v>0.88</v>
       </c>
       <c r="Z51">
-        <v>3.5000000000000003E-2</v>
+        <v>0.124</v>
       </c>
       <c r="AA51">
-        <v>0.36799999999999999</v>
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="AB51">
+        <v>23.2</v>
       </c>
       <c r="AC51">
-        <v>2</v>
+        <v>400</v>
       </c>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="C52">
-        <v>0.32</v>
+        <v>3</v>
       </c>
       <c r="D52">
-        <v>99.7</v>
+        <v>77</v>
       </c>
       <c r="E52">
-        <v>99.7</v>
+        <v>40</v>
       </c>
       <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="I52">
-        <v>1.9E-2</v>
+        <v>7</v>
       </c>
       <c r="T52">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="U52">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="X52">
-        <v>0.05</v>
-      </c>
-      <c r="Y52">
-        <v>0.01</v>
-      </c>
-      <c r="Z52">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AB52">
-        <v>0.6</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="AC52">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B53">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C53">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="D53">
-        <v>3.9</v>
+        <v>7.96</v>
       </c>
       <c r="E53">
-        <v>2.6</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="F53">
-        <v>0.9</v>
-      </c>
-      <c r="G53">
-        <v>42</v>
-      </c>
-      <c r="H53">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="I53">
-        <v>1.9E-2</v>
-      </c>
-      <c r="J53">
-        <v>0.59399999999999997</v>
-      </c>
-      <c r="K53">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="L53">
-        <v>0.08</v>
+        <v>0.64</v>
       </c>
       <c r="M53">
-        <v>0.7</v>
-      </c>
-      <c r="N53">
-        <v>15</v>
+        <v>3.7</v>
       </c>
       <c r="P53">
-        <v>13.7</v>
-      </c>
-      <c r="R53">
-        <v>0.54</v>
-      </c>
-      <c r="S53">
-        <v>7.9</v>
+        <v>59.6</v>
       </c>
       <c r="T53">
-        <v>237</v>
+        <v>161</v>
       </c>
       <c r="U53">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="V53">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W53">
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="X53">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="Y53">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
       <c r="Z53">
-        <v>5.8999999999999997E-2</v>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA53">
+        <v>0.36799999999999999</v>
       </c>
       <c r="AC53">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="B54">
-        <v>884</v>
+        <v>385</v>
       </c>
       <c r="C54">
-        <v>100</v>
+        <v>0.32</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>99.7</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>99.7</v>
       </c>
       <c r="F54">
         <v>0</v>
       </c>
+      <c r="I54">
+        <v>1.9E-2</v>
+      </c>
+      <c r="T54">
+        <v>2</v>
+      </c>
+      <c r="U54">
+        <v>1</v>
+      </c>
+      <c r="X54">
+        <v>0.05</v>
+      </c>
+      <c r="Y54">
+        <v>0.01</v>
+      </c>
+      <c r="Z54">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AB54">
+        <v>0.6</v>
+      </c>
+      <c r="AC54">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="B55">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="C55">
-        <v>4.4800000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="D55">
-        <v>5.57</v>
+        <v>3.9</v>
       </c>
       <c r="E55">
-        <v>4.09</v>
+        <v>2.6</v>
       </c>
       <c r="F55">
-        <v>3.82</v>
+        <v>0.9</v>
       </c>
       <c r="G55">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H55">
-        <v>5.5E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="I55">
-        <v>0.24299999999999999</v>
+        <v>1.9E-2</v>
       </c>
       <c r="J55">
-        <v>0.13500000000000001</v>
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="K55">
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="L55">
-        <v>4.4999999999999998E-2</v>
+        <v>0.08</v>
       </c>
       <c r="M55">
-        <v>3</v>
-      </c>
-      <c r="Q55">
-        <v>0.78</v>
+        <v>0.7</v>
+      </c>
+      <c r="N55">
+        <v>15</v>
+      </c>
+      <c r="P55">
+        <v>13.7</v>
+      </c>
+      <c r="R55">
+        <v>0.54</v>
       </c>
       <c r="S55">
-        <v>0.2</v>
+        <v>7.9</v>
       </c>
       <c r="T55">
-        <v>164</v>
+        <v>237</v>
       </c>
       <c r="U55">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="V55">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="W55">
-        <v>11.4</v>
+        <v>11</v>
       </c>
       <c r="X55">
-        <v>0.05</v>
+        <v>0.27</v>
       </c>
       <c r="Y55">
-        <v>0.43</v>
+        <v>0.17</v>
       </c>
       <c r="Z55">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AA55">
-        <v>2E-3</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC55">
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56">
+        <v>884</v>
+      </c>
+      <c r="C56">
+        <v>100</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57">
+        <v>18</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58">
+        <v>78</v>
+      </c>
+      <c r="C58">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="D58">
+        <v>5.57</v>
+      </c>
+      <c r="E58">
+        <v>4.09</v>
+      </c>
+      <c r="F58">
+        <v>3.82</v>
+      </c>
+      <c r="G58">
+        <v>48</v>
+      </c>
+      <c r="H58">
+        <v>5.5E-2</v>
+      </c>
+      <c r="I58">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="J58">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L58">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M58">
+        <v>3</v>
+      </c>
+      <c r="Q58">
+        <v>0.78</v>
+      </c>
+      <c r="S58">
+        <v>0.2</v>
+      </c>
+      <c r="T58">
+        <v>164</v>
+      </c>
+      <c r="U58">
+        <v>127</v>
+      </c>
+      <c r="V58">
+        <v>101</v>
+      </c>
+      <c r="W58">
+        <v>11.4</v>
+      </c>
+      <c r="X58">
+        <v>0.05</v>
+      </c>
+      <c r="Y58">
+        <v>0.43</v>
+      </c>
+      <c r="Z58">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AA58">
+        <v>2E-3</v>
+      </c>
+      <c r="AC58">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B56">
+      <c r="B59">
         <v>19.8</v>
       </c>
-      <c r="C56">
+      <c r="C59">
         <v>0.22</v>
       </c>
-      <c r="D56">
+      <c r="D59">
         <v>4.1500000000000004</v>
       </c>
-      <c r="E56">
+      <c r="E59">
         <v>2.15</v>
       </c>
-      <c r="F56">
+      <c r="F59">
         <v>1.5</v>
       </c>
     </row>
@@ -3355,7 +3594,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G56">
+  <conditionalFormatting sqref="G4:G59 H47:AC47">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -3367,7 +3606,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G57:G1048576 G1:G52 H53:H56">
+  <conditionalFormatting sqref="G60:G1048576 G1:G54 H55:H59 H47:AC47">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -3379,7 +3618,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H57:H1048576 H1:H52 I53:I56">
+  <conditionalFormatting sqref="H60:H1048576 H1:H46 I55:I59 H48:H54">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -3391,7 +3630,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I57:I1048576 I1:I52 J53:J56">
+  <conditionalFormatting sqref="I60:I1048576 I1:I46 J55:J59 I48:I54">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -3403,7 +3642,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J57:J1048576 J1:J52">
+  <conditionalFormatting sqref="J60:J1048576 J1:J46 J48:J54">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -3415,7 +3654,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
+  <conditionalFormatting sqref="K48:K1048576 K1:K46">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -3427,7 +3666,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1048576">
+  <conditionalFormatting sqref="L48:L1048576 L1:L46">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -3439,7 +3678,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1048576">
+  <conditionalFormatting sqref="M48:M1048576 M1:M46">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -3451,7 +3690,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576">
+  <conditionalFormatting sqref="N48:N1048576 N1:N46">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -3463,7 +3702,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1048576">
+  <conditionalFormatting sqref="O48:O1048576 O1:O46">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3475,7 +3714,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048576">
+  <conditionalFormatting sqref="P48:P1048576 P1:P46">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -3487,7 +3726,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q1048576">
+  <conditionalFormatting sqref="Q48:Q1048576 Q1:Q46">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3499,7 +3738,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R1048576">
+  <conditionalFormatting sqref="R48:R1048576 R1:R46">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -3511,7 +3750,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S1048576">
+  <conditionalFormatting sqref="S48:S1048576 S1:S46">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3523,7 +3762,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T1:T1048576">
+  <conditionalFormatting sqref="T48:T1048576 T1:T46">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -3535,7 +3774,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U1048576">
+  <conditionalFormatting sqref="U48:U1048576 U1:U46">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -3547,7 +3786,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:V1048576">
+  <conditionalFormatting sqref="V48:V1048576 V1:V46">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3559,7 +3798,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W1:W1048576">
+  <conditionalFormatting sqref="W48:W1048576 W1:W46">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -3571,7 +3810,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X1:X1048576">
+  <conditionalFormatting sqref="X48:X1048576 X1:X46">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -3583,7 +3822,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y1:Y1048576">
+  <conditionalFormatting sqref="Y48:Y1048576 Y1:Y46">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3595,7 +3834,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z1:Z1048576">
+  <conditionalFormatting sqref="Z48:Z1048576 Z1:Z46">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3607,7 +3846,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA1:AA1048576">
+  <conditionalFormatting sqref="AA48:AA1048576 AA1:AA46">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3619,7 +3858,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB1:AB1048576">
+  <conditionalFormatting sqref="AB48:AB1048576 AB1:AB46">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3631,7 +3870,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC1:AC1048576">
+  <conditionalFormatting sqref="AC48:AC1048576 AC1:AC46">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Recipe Churros de pescado and minor fixes
</commit_message>
<xml_diff>
--- a/assets/data/recipes/foodProperties.xlsx
+++ b/assets/data/recipes/foodProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1pab\Desktop\Pablo\showtime\assets\data\recipes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B16EA09-E9FF-4B0E-A638-D6D1E66D617A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53D74D2-DEDC-4EFA-9C00-411E8AEF9EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="105">
   <si>
     <t>Ingredient</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>cilantro</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>merluza</t>
   </si>
 </sst>
 </file>
@@ -708,13 +714,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC59"/>
+  <dimension ref="A1:AC61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="29" ySplit="3" topLeftCell="AD4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="29" ySplit="3" topLeftCell="AE40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AD1" sqref="AD1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S19" sqref="S19"/>
+      <selection pane="bottomRight" activeCell="U64" sqref="U64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,273 +1359,273 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="B10">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C10">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>6.7</v>
+        <v>3.6</v>
       </c>
       <c r="E10">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0.88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="B11">
-        <v>266</v>
+        <v>32</v>
       </c>
       <c r="C11">
-        <v>3.29</v>
+        <v>0.16</v>
       </c>
       <c r="D11">
-        <v>50.61</v>
+        <v>6.7</v>
       </c>
       <c r="E11">
-        <v>4.3099999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="F11">
-        <v>7.64</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B12">
-        <v>717</v>
+        <v>266</v>
       </c>
       <c r="C12">
-        <v>81.099999999999994</v>
+        <v>3.29</v>
       </c>
       <c r="D12">
-        <v>0.06</v>
+        <v>50.61</v>
       </c>
       <c r="E12">
-        <v>0.06</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="F12">
-        <v>0.85</v>
+        <v>7.64</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B13">
-        <v>25</v>
+        <v>717</v>
       </c>
       <c r="C13">
-        <v>0.1</v>
+        <v>81.099999999999994</v>
       </c>
       <c r="D13">
-        <v>5.8</v>
+        <v>0.06</v>
       </c>
       <c r="E13">
-        <v>3.2</v>
+        <v>0.06</v>
       </c>
       <c r="F13">
-        <v>1.28</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B14">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C14">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="D14">
-        <v>10.3</v>
+        <v>5.8</v>
       </c>
       <c r="E14">
-        <v>4.7</v>
+        <v>3.2</v>
       </c>
       <c r="F14">
-        <v>0.94</v>
-      </c>
-      <c r="G14">
-        <v>835</v>
-      </c>
-      <c r="H14">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="I14">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="J14">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="K14">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="L14">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="N14">
-        <v>19</v>
-      </c>
-      <c r="P14">
-        <v>5.9</v>
-      </c>
-      <c r="R14">
-        <v>0.66</v>
-      </c>
-      <c r="S14">
-        <v>13.2</v>
-      </c>
-      <c r="T14">
-        <v>320</v>
-      </c>
-      <c r="U14">
-        <v>33</v>
-      </c>
-      <c r="V14">
-        <v>35</v>
-      </c>
-      <c r="W14">
-        <v>12</v>
-      </c>
-      <c r="X14">
-        <v>0.3</v>
-      </c>
-      <c r="Y14">
-        <v>0.24</v>
-      </c>
-      <c r="Z14">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA14">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="AB14">
-        <v>0.1</v>
-      </c>
-      <c r="AC14">
-        <v>69</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C15">
-        <v>0.17</v>
+        <v>0.35</v>
       </c>
       <c r="D15">
-        <v>2.97</v>
+        <v>10.3</v>
       </c>
       <c r="E15">
-        <v>1.34</v>
+        <v>4.7</v>
       </c>
       <c r="F15">
-        <v>0.69</v>
+        <v>0.94</v>
       </c>
       <c r="G15">
-        <v>22</v>
+        <v>835</v>
       </c>
       <c r="H15">
-        <v>2.1000000000000001E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="I15">
-        <v>5.7000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="J15">
-        <v>0.32</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="K15">
-        <v>0.246</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="L15">
-        <v>7.3999999999999996E-2</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="N15">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="P15">
-        <v>3.1</v>
+        <v>5.9</v>
       </c>
       <c r="R15">
-        <v>0.27</v>
+        <v>0.66</v>
       </c>
       <c r="S15">
-        <v>29.3</v>
+        <v>13.2</v>
       </c>
       <c r="T15">
-        <v>260</v>
+        <v>320</v>
       </c>
       <c r="U15">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="V15">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="W15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X15">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="Y15">
-        <v>0.13</v>
+        <v>0.24</v>
       </c>
       <c r="Z15">
-        <v>3.5000000000000003E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AA15">
-        <v>0.10299999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="AB15">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="AC15">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B16">
-        <v>239</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>0.17</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2.97</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="F16">
-        <v>27</v>
+        <v>0.69</v>
+      </c>
+      <c r="G16">
+        <v>22</v>
+      </c>
+      <c r="H16">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I16">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="J16">
+        <v>0.32</v>
+      </c>
+      <c r="K16">
+        <v>0.246</v>
+      </c>
+      <c r="L16">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="N16">
+        <v>36</v>
+      </c>
+      <c r="P16">
+        <v>3.1</v>
+      </c>
+      <c r="R16">
+        <v>0.27</v>
+      </c>
+      <c r="S16">
+        <v>29.3</v>
+      </c>
+      <c r="T16">
+        <v>260</v>
+      </c>
+      <c r="U16">
+        <v>40</v>
+      </c>
+      <c r="V16">
+        <v>24</v>
+      </c>
+      <c r="W16">
+        <v>11</v>
+      </c>
+      <c r="X16">
+        <v>0.2</v>
+      </c>
+      <c r="Y16">
+        <v>0.13</v>
+      </c>
+      <c r="Z16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA16">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="AB16">
+        <v>0.4</v>
+      </c>
+      <c r="AC16">
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="B17">
-        <v>106</v>
+        <v>239</v>
       </c>
       <c r="C17">
-        <v>1.93</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1628,1016 +1634,1013 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>22.5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="B18">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C18">
-        <v>1.7</v>
+        <v>1.93</v>
       </c>
       <c r="D18">
-        <v>14.2</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>6.9</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B19">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="C19">
-        <v>0.6</v>
+        <v>1.7</v>
       </c>
       <c r="D19">
-        <v>1.9</v>
+        <v>14.2</v>
       </c>
       <c r="E19">
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="F19">
-        <v>3.1</v>
-      </c>
-      <c r="G19">
-        <v>515</v>
-      </c>
-      <c r="H19">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="I19">
-        <v>0.185</v>
-      </c>
-      <c r="J19">
-        <v>0.2</v>
-      </c>
-      <c r="K19">
-        <v>0.54</v>
-      </c>
-      <c r="L19">
-        <v>0.08</v>
-      </c>
-      <c r="N19">
-        <v>0.126</v>
-      </c>
-      <c r="P19">
-        <v>30</v>
-      </c>
-      <c r="R19">
-        <v>1.7</v>
-      </c>
-      <c r="T19">
-        <v>540</v>
-      </c>
-      <c r="U19">
-        <v>86</v>
-      </c>
-      <c r="V19">
-        <v>54</v>
-      </c>
-      <c r="W19">
-        <v>30</v>
-      </c>
-      <c r="X19">
-        <v>4.5</v>
-      </c>
-      <c r="Y19">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="Z19">
-        <v>0.09</v>
-      </c>
-      <c r="AA19">
-        <v>0.47</v>
-      </c>
-      <c r="AC19">
-        <v>45</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B20">
-        <v>579</v>
+        <v>26</v>
       </c>
       <c r="C20">
-        <v>38.299999999999997</v>
+        <v>0.6</v>
       </c>
       <c r="D20">
-        <v>52.4</v>
+        <v>1.9</v>
       </c>
       <c r="E20">
-        <v>36.700000000000003</v>
+        <v>1.2</v>
       </c>
       <c r="F20">
-        <v>6.12</v>
+        <v>3.1</v>
+      </c>
+      <c r="G20">
+        <v>515</v>
+      </c>
+      <c r="H20">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="I20">
+        <v>0.185</v>
       </c>
       <c r="J20">
-        <v>0.83799999999999997</v>
+        <v>0.2</v>
       </c>
       <c r="K20">
-        <v>0.3</v>
+        <v>0.54</v>
+      </c>
+      <c r="L20">
+        <v>0.08</v>
+      </c>
+      <c r="N20">
+        <v>0.126</v>
+      </c>
+      <c r="P20">
+        <v>30</v>
       </c>
       <c r="R20">
-        <v>0.59</v>
-      </c>
-      <c r="S20">
-        <v>7.2</v>
+        <v>1.7</v>
       </c>
       <c r="T20">
-        <v>567</v>
+        <v>540</v>
       </c>
       <c r="U20">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="V20">
-        <v>260</v>
+        <v>54</v>
       </c>
       <c r="W20">
-        <v>176</v>
+        <v>30</v>
       </c>
       <c r="X20">
-        <v>6.32</v>
+        <v>4.5</v>
       </c>
       <c r="Y20">
-        <v>2.65</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z20">
-        <v>1.25</v>
+        <v>0.09</v>
       </c>
       <c r="AA20">
-        <v>1.32</v>
-      </c>
-      <c r="AB20">
-        <v>8.4</v>
+        <v>0.47</v>
       </c>
       <c r="AC20">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B21">
-        <v>333</v>
+        <v>579</v>
       </c>
       <c r="C21">
-        <v>29.18</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="D21">
-        <v>2.85</v>
+        <v>52.4</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="F21">
-        <v>13.72</v>
+        <v>6.12</v>
+      </c>
+      <c r="J21">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="K21">
+        <v>0.3</v>
+      </c>
+      <c r="R21">
+        <v>0.59</v>
+      </c>
+      <c r="S21">
+        <v>7.2</v>
+      </c>
+      <c r="T21">
+        <v>567</v>
+      </c>
+      <c r="U21">
+        <v>62</v>
+      </c>
+      <c r="V21">
+        <v>260</v>
+      </c>
+      <c r="W21">
+        <v>176</v>
+      </c>
+      <c r="X21">
+        <v>6.32</v>
+      </c>
+      <c r="Y21">
+        <v>2.65</v>
+      </c>
+      <c r="Z21">
+        <v>1.25</v>
+      </c>
+      <c r="AA21">
+        <v>1.32</v>
+      </c>
+      <c r="AB21">
+        <v>8.4</v>
+      </c>
+      <c r="AC21">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B22">
-        <v>86</v>
+        <v>333</v>
       </c>
       <c r="C22">
-        <v>1.35</v>
+        <v>29.18</v>
       </c>
       <c r="D22">
-        <v>18.7</v>
+        <v>2.85</v>
       </c>
       <c r="E22">
-        <v>6.26</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>3.27</v>
+        <v>13.72</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B23">
-        <v>228</v>
+        <v>86</v>
       </c>
       <c r="C23">
-        <v>13.7</v>
+        <v>1.35</v>
       </c>
       <c r="D23">
-        <v>57.9</v>
+        <v>18.7</v>
       </c>
       <c r="E23">
-        <v>1.75</v>
+        <v>6.26</v>
       </c>
       <c r="F23">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I23">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="J23">
-        <v>2.1850000000000001</v>
-      </c>
-      <c r="N23">
-        <v>32</v>
-      </c>
-      <c r="S23">
-        <v>2.5</v>
-      </c>
-      <c r="T23">
-        <v>1525</v>
-      </c>
-      <c r="U23">
-        <v>128</v>
-      </c>
-      <c r="V23">
-        <v>734</v>
-      </c>
-      <c r="W23">
-        <v>499</v>
-      </c>
-      <c r="X23">
-        <v>13.86</v>
-      </c>
-      <c r="Y23">
-        <v>6.81</v>
-      </c>
-      <c r="Z23">
-        <v>3.7879999999999998</v>
-      </c>
-      <c r="AA23">
-        <v>3.3849999999999998</v>
-      </c>
-      <c r="AB23">
-        <v>14.3</v>
-      </c>
-      <c r="AC23">
-        <v>21</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B24">
-        <v>350</v>
+        <v>228</v>
       </c>
       <c r="C24">
-        <v>34.4</v>
+        <v>13.7</v>
       </c>
       <c r="D24">
-        <v>5.52</v>
+        <v>57.9</v>
       </c>
       <c r="E24">
-        <v>3.76</v>
+        <v>1.75</v>
       </c>
       <c r="F24">
-        <v>6.15</v>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="I24">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="J24">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="N24">
+        <v>32</v>
+      </c>
+      <c r="S24">
+        <v>2.5</v>
+      </c>
+      <c r="T24">
+        <v>1525</v>
+      </c>
+      <c r="U24">
+        <v>128</v>
+      </c>
+      <c r="V24">
+        <v>734</v>
+      </c>
+      <c r="W24">
+        <v>499</v>
+      </c>
+      <c r="X24">
+        <v>13.86</v>
+      </c>
+      <c r="Y24">
+        <v>6.81</v>
+      </c>
+      <c r="Z24">
+        <v>3.7879999999999998</v>
+      </c>
+      <c r="AA24">
+        <v>3.3849999999999998</v>
+      </c>
+      <c r="AB24">
+        <v>14.3</v>
+      </c>
+      <c r="AC24">
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B25">
-        <v>15</v>
+        <v>350</v>
       </c>
       <c r="C25">
-        <v>0.1</v>
+        <v>34.4</v>
       </c>
       <c r="D25">
-        <v>3.6</v>
+        <v>5.52</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>3.76</v>
       </c>
       <c r="F25">
-        <v>0.7</v>
+        <v>6.15</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B26">
-        <v>420</v>
+        <v>15</v>
       </c>
       <c r="C26">
-        <v>27.8</v>
+        <v>0.1</v>
       </c>
       <c r="D26">
-        <v>13.9</v>
+        <v>3.6</v>
       </c>
       <c r="E26">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>28.4</v>
-      </c>
-      <c r="G26">
-        <v>262</v>
-      </c>
-      <c r="H26">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="I26">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="J26">
-        <v>0.08</v>
-      </c>
-      <c r="K26">
-        <v>0.45</v>
-      </c>
-      <c r="L26">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="N26">
-        <v>6</v>
-      </c>
-      <c r="O26">
-        <v>1.4</v>
-      </c>
-      <c r="Q26">
-        <v>0.5</v>
-      </c>
-      <c r="R26">
-        <v>0.53</v>
-      </c>
-      <c r="S26">
-        <v>1.7</v>
-      </c>
-      <c r="T26">
-        <v>180</v>
-      </c>
-      <c r="U26">
-        <v>853</v>
-      </c>
-      <c r="V26">
-        <v>627</v>
-      </c>
-      <c r="W26">
-        <v>34</v>
-      </c>
-      <c r="X26">
-        <v>0.49</v>
-      </c>
-      <c r="Y26">
-        <v>4.2</v>
-      </c>
-      <c r="Z26">
-        <v>0.04</v>
-      </c>
-      <c r="AA26">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="AB26">
-        <v>34.4</v>
-      </c>
-      <c r="AC26">
-        <v>1800</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B27">
-        <v>142</v>
+        <v>420</v>
       </c>
       <c r="C27">
-        <v>9.9600000000000009</v>
+        <v>27.8</v>
       </c>
       <c r="D27">
-        <v>0.96</v>
+        <v>13.9</v>
       </c>
       <c r="E27">
-        <v>0.2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F27">
-        <v>12.4</v>
-      </c>
-      <c r="M27">
-        <v>21</v>
+        <v>28.4</v>
+      </c>
+      <c r="G27">
+        <v>262</v>
+      </c>
+      <c r="H27">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I27">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="J27">
+        <v>0.08</v>
+      </c>
+      <c r="K27">
+        <v>0.45</v>
+      </c>
+      <c r="L27">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="N27">
+        <v>6</v>
+      </c>
+      <c r="O27">
+        <v>1.4</v>
+      </c>
+      <c r="Q27">
+        <v>0.5</v>
+      </c>
+      <c r="R27">
+        <v>0.53</v>
+      </c>
+      <c r="S27">
+        <v>1.7</v>
+      </c>
+      <c r="T27">
+        <v>180</v>
+      </c>
+      <c r="U27">
+        <v>853</v>
+      </c>
+      <c r="V27">
+        <v>627</v>
+      </c>
+      <c r="W27">
+        <v>34</v>
+      </c>
+      <c r="X27">
+        <v>0.49</v>
+      </c>
+      <c r="Y27">
+        <v>4.2</v>
+      </c>
+      <c r="Z27">
+        <v>0.04</v>
+      </c>
+      <c r="AA27">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="AB27">
+        <v>34.4</v>
+      </c>
+      <c r="AC27">
+        <v>1800</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28">
-        <v>322</v>
+        <v>142</v>
       </c>
       <c r="C28">
-        <v>26.5</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="D28">
-        <v>3.59</v>
+        <v>0.96</v>
       </c>
       <c r="E28">
-        <v>0.56000000000000005</v>
+        <v>0.2</v>
       </c>
       <c r="F28">
-        <v>15.9</v>
-      </c>
-      <c r="G28">
-        <v>381</v>
-      </c>
-      <c r="H28">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="I28">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="J28">
-        <v>2.4E-2</v>
-      </c>
-      <c r="K28">
-        <v>2.99</v>
-      </c>
-      <c r="L28">
-        <v>0.35</v>
+        <v>12.4</v>
       </c>
       <c r="M28">
-        <v>27</v>
-      </c>
-      <c r="N28">
-        <v>146</v>
-      </c>
-      <c r="O28">
-        <v>1.95</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <v>5.4</v>
-      </c>
-      <c r="R28">
-        <v>2.58</v>
-      </c>
-      <c r="S28">
-        <v>0.7</v>
-      </c>
-      <c r="T28">
-        <v>109</v>
-      </c>
-      <c r="U28">
-        <v>129</v>
-      </c>
-      <c r="V28">
-        <v>390</v>
-      </c>
-      <c r="W28">
-        <v>5</v>
-      </c>
-      <c r="X28">
-        <v>2.73</v>
-      </c>
-      <c r="Y28">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="Z28">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="AA28">
-        <v>5.5E-2</v>
-      </c>
-      <c r="AB28">
-        <v>56</v>
-      </c>
-      <c r="AC28">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="B29">
-        <v>364</v>
+        <v>322</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>26.5</v>
       </c>
       <c r="D29">
-        <v>76.3</v>
+        <v>3.59</v>
       </c>
       <c r="E29">
-        <v>0.3</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F29">
-        <v>10</v>
+        <v>15.9</v>
+      </c>
+      <c r="G29">
+        <v>381</v>
+      </c>
+      <c r="H29">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I29">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="J29">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K29">
+        <v>2.99</v>
+      </c>
+      <c r="L29">
+        <v>0.35</v>
+      </c>
+      <c r="M29">
+        <v>27</v>
+      </c>
+      <c r="N29">
+        <v>146</v>
+      </c>
+      <c r="O29">
+        <v>1.95</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>5.4</v>
+      </c>
+      <c r="R29">
+        <v>2.58</v>
+      </c>
+      <c r="S29">
+        <v>0.7</v>
       </c>
       <c r="T29">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="U29">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="V29">
-        <v>108</v>
+        <v>390</v>
       </c>
       <c r="W29">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="X29">
-        <v>1.17</v>
+        <v>2.73</v>
       </c>
       <c r="Y29">
-        <v>0.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Z29">
-        <v>0.14399999999999999</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="AA29">
-        <v>0.68200000000000005</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AB29">
-        <v>33.9</v>
+        <v>56</v>
       </c>
       <c r="AC29">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="B30">
-        <v>143</v>
+        <v>364</v>
       </c>
       <c r="C30">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>28.2</v>
+        <v>76.3</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F30">
-        <v>6.62</v>
+        <v>10</v>
+      </c>
+      <c r="T30">
+        <v>107</v>
+      </c>
+      <c r="U30">
+        <v>15</v>
+      </c>
+      <c r="V30">
+        <v>108</v>
+      </c>
+      <c r="W30">
+        <v>22</v>
+      </c>
+      <c r="X30">
+        <v>1.17</v>
+      </c>
+      <c r="Y30">
+        <v>0.7</v>
+      </c>
+      <c r="Z30">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="AA30">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="AB30">
+        <v>33.9</v>
+      </c>
+      <c r="AC30">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31">
-        <v>357</v>
+        <v>143</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>28.2</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31">
-        <v>89</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="B32">
-        <v>379</v>
+        <v>357</v>
       </c>
       <c r="C32">
-        <v>4.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>72.8</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>3.38</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>7.95</v>
-      </c>
-      <c r="AC32">
-        <v>0.49</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B33">
-        <v>35</v>
+        <v>379</v>
       </c>
       <c r="C33">
-        <v>0.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D33">
-        <v>7.9</v>
+        <v>72.8</v>
       </c>
       <c r="E33">
-        <v>3.6</v>
+        <v>3.38</v>
       </c>
       <c r="F33">
-        <v>1.9</v>
+        <v>7.95</v>
+      </c>
+      <c r="AC33">
+        <v>0.49</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B34">
-        <v>655</v>
+        <v>35</v>
       </c>
       <c r="C34">
-        <v>69.61</v>
+        <v>0.3</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="F34">
-        <v>6.38</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B35">
-        <v>340</v>
+        <v>655</v>
       </c>
       <c r="C35">
-        <v>36.1</v>
+        <v>69.61</v>
       </c>
       <c r="D35">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>2.84</v>
-      </c>
-      <c r="G35">
-        <v>411</v>
-      </c>
-      <c r="H35">
-        <v>0.02</v>
-      </c>
-      <c r="I35">
-        <v>0.188</v>
-      </c>
-      <c r="J35">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="L35">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="N35">
-        <v>4</v>
-      </c>
-      <c r="O35">
-        <v>0.16</v>
-      </c>
-      <c r="P35">
-        <v>0.6</v>
-      </c>
-      <c r="Q35">
-        <v>1.6</v>
-      </c>
-      <c r="R35">
-        <v>0.92</v>
-      </c>
-      <c r="S35">
-        <v>3.2</v>
-      </c>
-      <c r="T35">
-        <v>95</v>
-      </c>
-      <c r="U35">
-        <v>66</v>
-      </c>
-      <c r="V35">
-        <v>58</v>
-      </c>
-      <c r="W35">
-        <v>7</v>
-      </c>
-      <c r="X35">
-        <v>0.1</v>
-      </c>
-      <c r="Y35">
-        <v>0.24</v>
-      </c>
-      <c r="Z35">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="AB35">
-        <v>3</v>
-      </c>
-      <c r="AC35">
-        <v>27</v>
+        <v>6.38</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36">
-        <v>61</v>
+        <v>340</v>
       </c>
       <c r="C36">
-        <v>0.3</v>
+        <v>36.1</v>
       </c>
       <c r="D36">
-        <v>14</v>
+        <v>2.9</v>
       </c>
       <c r="E36">
-        <v>3.9</v>
+        <v>2.9</v>
       </c>
       <c r="F36">
-        <v>1.5</v>
+        <v>2.84</v>
+      </c>
+      <c r="G36">
+        <v>411</v>
+      </c>
+      <c r="H36">
+        <v>0.02</v>
+      </c>
+      <c r="I36">
+        <v>0.188</v>
+      </c>
+      <c r="J36">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L36">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N36">
+        <v>4</v>
+      </c>
+      <c r="O36">
+        <v>0.16</v>
+      </c>
+      <c r="P36">
+        <v>0.6</v>
+      </c>
+      <c r="Q36">
+        <v>1.6</v>
+      </c>
+      <c r="R36">
+        <v>0.92</v>
+      </c>
+      <c r="S36">
+        <v>3.2</v>
+      </c>
+      <c r="T36">
+        <v>95</v>
+      </c>
+      <c r="U36">
+        <v>66</v>
+      </c>
+      <c r="V36">
+        <v>58</v>
+      </c>
+      <c r="W36">
+        <v>7</v>
+      </c>
+      <c r="X36">
+        <v>0.1</v>
+      </c>
+      <c r="Y36">
+        <v>0.24</v>
+      </c>
+      <c r="Z36">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AB36">
+        <v>3</v>
+      </c>
+      <c r="AC36">
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B37">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C37">
-        <v>0.38</v>
+        <v>0.3</v>
       </c>
       <c r="D37">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37">
-        <v>13.7</v>
+        <v>3.9</v>
       </c>
       <c r="F37">
-        <v>0.82</v>
-      </c>
-      <c r="G37">
-        <v>54</v>
-      </c>
-      <c r="H37">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="I37">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="J37">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="K37">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="L37">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="N37">
-        <v>43</v>
-      </c>
-      <c r="P37">
-        <v>36.4</v>
-      </c>
-      <c r="S37">
-        <v>4.2</v>
-      </c>
-      <c r="T37">
-        <v>168</v>
-      </c>
-      <c r="U37">
-        <v>11</v>
-      </c>
-      <c r="V37">
-        <v>14</v>
-      </c>
-      <c r="W37">
-        <v>10</v>
-      </c>
-      <c r="X37">
-        <v>0.16</v>
-      </c>
-      <c r="Y37">
-        <v>0.09</v>
-      </c>
-      <c r="Z37">
-        <v>0.111</v>
-      </c>
-      <c r="AA37">
-        <v>6.3E-2</v>
-      </c>
-      <c r="AB37">
-        <v>0.6</v>
-      </c>
-      <c r="AC37">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B38">
-        <v>429</v>
+        <v>60</v>
       </c>
       <c r="C38">
-        <v>50</v>
+        <v>0.38</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>13.7</v>
       </c>
       <c r="F38">
-        <v>7.14</v>
+        <v>0.82</v>
+      </c>
+      <c r="G38">
+        <v>54</v>
+      </c>
+      <c r="H38">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I38">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J38">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="K38">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="L38">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="N38">
+        <v>43</v>
+      </c>
+      <c r="P38">
+        <v>36.4</v>
+      </c>
+      <c r="S38">
+        <v>4.2</v>
+      </c>
+      <c r="T38">
+        <v>168</v>
       </c>
       <c r="U38">
-        <v>143</v>
+        <v>11</v>
+      </c>
+      <c r="V38">
+        <v>14</v>
+      </c>
+      <c r="W38">
+        <v>10</v>
+      </c>
+      <c r="X38">
+        <v>0.16</v>
+      </c>
+      <c r="Y38">
+        <v>0.09</v>
+      </c>
+      <c r="Z38">
+        <v>0.111</v>
+      </c>
+      <c r="AA38">
+        <v>6.3E-2</v>
+      </c>
+      <c r="AB38">
+        <v>0.6</v>
       </c>
       <c r="AC38">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39">
-        <v>61</v>
+        <v>429</v>
       </c>
       <c r="C39">
-        <v>3.2</v>
+        <v>50</v>
       </c>
       <c r="D39">
-        <v>4.9000000000000004</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>4.9000000000000004</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>3.27</v>
-      </c>
-      <c r="G39">
-        <v>32</v>
-      </c>
-      <c r="H39">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="I39">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="J39">
-        <v>0.105</v>
-      </c>
-      <c r="L39">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="M39">
-        <v>0.1</v>
-      </c>
-      <c r="O39">
-        <v>0.54</v>
-      </c>
-      <c r="R39">
-        <v>0.05</v>
-      </c>
-      <c r="S39">
-        <v>0.3</v>
-      </c>
-      <c r="T39">
-        <v>150</v>
+        <v>7.14</v>
       </c>
       <c r="U39">
-        <v>123</v>
-      </c>
-      <c r="V39">
-        <v>101</v>
-      </c>
-      <c r="W39">
-        <v>12</v>
-      </c>
-      <c r="Y39">
-        <v>0.41</v>
-      </c>
-      <c r="Z39">
-        <v>1E-3</v>
-      </c>
-      <c r="AB39">
-        <v>1.9</v>
+        <v>143</v>
       </c>
       <c r="AC39">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B40">
-        <v>379</v>
+        <v>73</v>
       </c>
       <c r="C40">
-        <v>34.5</v>
+        <v>1.2</v>
       </c>
       <c r="D40">
-        <v>1.29</v>
+        <v>0.2</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>14.6</v>
+        <v>15.2</v>
+      </c>
+      <c r="T40">
+        <v>306</v>
+      </c>
+      <c r="V40">
+        <v>154</v>
+      </c>
+      <c r="Y40">
+        <v>0.23</v>
+      </c>
+      <c r="AB40">
+        <v>47</v>
+      </c>
+      <c r="AC40">
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41">
-        <v>884</v>
+        <v>61</v>
       </c>
       <c r="C41">
-        <v>100</v>
+        <v>3.2</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>3.27</v>
+      </c>
+      <c r="G41">
+        <v>32</v>
+      </c>
+      <c r="H41">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I41">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="J41">
+        <v>0.105</v>
+      </c>
+      <c r="L41">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M41">
+        <v>0.1</v>
+      </c>
+      <c r="O41">
+        <v>0.54</v>
       </c>
       <c r="R41">
-        <v>14.4</v>
+        <v>0.05</v>
       </c>
       <c r="S41">
-        <v>60.2</v>
+        <v>0.3</v>
       </c>
       <c r="T41">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="U41">
-        <v>1</v>
-      </c>
-      <c r="X41">
-        <v>0.56000000000000005</v>
+        <v>123</v>
+      </c>
+      <c r="V41">
+        <v>101</v>
+      </c>
+      <c r="W41">
+        <v>12</v>
+      </c>
+      <c r="Y41">
+        <v>0.41</v>
+      </c>
+      <c r="Z41">
+        <v>1E-3</v>
+      </c>
+      <c r="AB41">
+        <v>1.9</v>
       </c>
       <c r="AC41">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="B42">
-        <v>36</v>
+        <v>379</v>
       </c>
       <c r="C42">
-        <v>0.13</v>
+        <v>34.5</v>
       </c>
       <c r="D42">
-        <v>7.68</v>
+        <v>1.29</v>
       </c>
       <c r="E42">
-        <v>5.76</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>0.89</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="B43">
-        <v>393</v>
+        <v>884</v>
       </c>
       <c r="C43">
-        <v>35.71</v>
+        <v>100</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2646,890 +2649,948 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>17.86</v>
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>14.4</v>
+      </c>
+      <c r="S43">
+        <v>60.2</v>
+      </c>
+      <c r="T43">
+        <v>1</v>
+      </c>
+      <c r="U43">
+        <v>1</v>
+      </c>
+      <c r="X43">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AC43">
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44">
-        <v>371</v>
+        <v>36</v>
       </c>
       <c r="C44">
-        <v>1.51</v>
+        <v>0.13</v>
       </c>
       <c r="D44">
-        <v>74.67</v>
+        <v>7.68</v>
       </c>
       <c r="E44">
-        <v>2.7</v>
+        <v>5.76</v>
       </c>
       <c r="F44">
-        <v>13.04</v>
-      </c>
-      <c r="H44">
-        <v>1</v>
-      </c>
-      <c r="I44">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="J44">
-        <v>5.36</v>
-      </c>
-      <c r="X44">
-        <v>3.21</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B45">
-        <v>673</v>
+        <v>393</v>
       </c>
       <c r="C45">
-        <v>68.400000000000006</v>
+        <v>35.71</v>
       </c>
       <c r="D45">
-        <v>13.1</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>3.59</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>13.7</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45">
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="I45">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="J45">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="K45">
-        <v>0.313</v>
-      </c>
-      <c r="L45">
-        <v>9.4E-2</v>
-      </c>
-      <c r="N45">
-        <v>34</v>
-      </c>
-      <c r="P45">
-        <v>0.8</v>
-      </c>
-      <c r="R45">
-        <v>9.33</v>
-      </c>
-      <c r="S45">
-        <v>53.9</v>
-      </c>
-      <c r="T45">
-        <v>597</v>
-      </c>
-      <c r="U45">
-        <v>16</v>
-      </c>
-      <c r="V45">
-        <v>575</v>
-      </c>
-      <c r="W45">
-        <v>251</v>
-      </c>
-      <c r="X45">
-        <v>5.53</v>
-      </c>
-      <c r="Y45">
-        <v>6.45</v>
-      </c>
-      <c r="Z45">
-        <v>1.32</v>
-      </c>
-      <c r="AA45">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="AB45">
-        <v>0.7</v>
-      </c>
-      <c r="AC45">
-        <v>2</v>
+        <v>17.86</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B46">
-        <v>263</v>
+        <v>371</v>
       </c>
       <c r="C46">
-        <v>21.2</v>
+        <v>1.51</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>74.67</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="F46">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="G46">
-        <v>2</v>
+        <v>13.04</v>
       </c>
       <c r="H46">
-        <v>0.73199999999999998</v>
+        <v>1</v>
       </c>
       <c r="I46">
-        <v>0.23499999999999999</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="J46">
-        <v>4.34</v>
-      </c>
-      <c r="K46">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="L46">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="N46">
-        <v>5</v>
-      </c>
-      <c r="O46">
-        <v>0.7</v>
-      </c>
-      <c r="P46">
-        <v>0.7</v>
-      </c>
-      <c r="T46">
-        <v>287</v>
-      </c>
-      <c r="U46">
-        <v>14</v>
-      </c>
-      <c r="V46">
-        <v>175</v>
-      </c>
-      <c r="W46">
-        <v>19</v>
+        <v>5.36</v>
       </c>
       <c r="X46">
-        <v>0.88</v>
-      </c>
-      <c r="Y46">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Z46">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA46">
-        <v>0.01</v>
-      </c>
-      <c r="AB46">
-        <v>24.6</v>
-      </c>
-      <c r="AC46">
-        <v>56</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="B47">
-        <v>180</v>
+        <v>673</v>
       </c>
       <c r="C47">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="D47">
+        <v>13.1</v>
+      </c>
+      <c r="E47">
+        <v>3.59</v>
+      </c>
+      <c r="F47">
+        <v>13.7</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="I47">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="J47">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="K47">
+        <v>0.313</v>
+      </c>
+      <c r="L47">
+        <v>9.4E-2</v>
+      </c>
+      <c r="N47">
+        <v>34</v>
+      </c>
+      <c r="P47">
+        <v>0.8</v>
+      </c>
+      <c r="R47">
+        <v>9.33</v>
+      </c>
+      <c r="S47">
+        <v>53.9</v>
+      </c>
+      <c r="T47">
+        <v>597</v>
+      </c>
+      <c r="U47">
         <v>16</v>
       </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>11</v>
-      </c>
-      <c r="G47">
-        <v>1.2</v>
-      </c>
-      <c r="H47">
-        <v>0.44</v>
-      </c>
-      <c r="I47">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J47">
-        <v>2.6</v>
-      </c>
-      <c r="K47">
-        <v>0.4</v>
-      </c>
-      <c r="L47">
-        <v>0.22</v>
-      </c>
-      <c r="N47">
-        <v>3</v>
-      </c>
-      <c r="O47">
-        <v>0.42</v>
-      </c>
-      <c r="P47">
-        <v>0.42</v>
-      </c>
-      <c r="T47">
-        <v>172</v>
-      </c>
-      <c r="U47">
-        <v>8.4</v>
-      </c>
       <c r="V47">
-        <v>105</v>
+        <v>575</v>
       </c>
       <c r="W47">
-        <v>11.4</v>
+        <v>251</v>
       </c>
       <c r="X47">
-        <v>0.5</v>
+        <v>5.53</v>
       </c>
       <c r="Y47">
+        <v>6.45</v>
+      </c>
+      <c r="Z47">
         <v>1.32</v>
       </c>
-      <c r="Z47">
-        <v>2.7E-2</v>
-      </c>
       <c r="AA47">
-        <v>6.0000000000000001E-3</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AB47">
-        <v>14.76</v>
+        <v>0.7</v>
       </c>
       <c r="AC47">
-        <v>33.6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B48">
-        <v>72</v>
+        <v>263</v>
       </c>
       <c r="C48">
-        <v>0.26</v>
+        <v>21.2</v>
       </c>
       <c r="D48">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>1.81</v>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
       </c>
       <c r="H48">
-        <v>5.0999999999999997E-2</v>
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="I48">
+        <v>0.23499999999999999</v>
       </c>
       <c r="J48">
-        <v>1.58</v>
+        <v>4.34</v>
+      </c>
+      <c r="K48">
+        <v>0.66800000000000004</v>
       </c>
       <c r="L48">
-        <v>0.14499999999999999</v>
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="N48">
+        <v>5</v>
+      </c>
+      <c r="O48">
+        <v>0.7</v>
       </c>
       <c r="P48">
-        <v>23.3</v>
-      </c>
-      <c r="S48">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="T48">
-        <v>446</v>
+        <v>287</v>
       </c>
       <c r="U48">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="V48">
-        <v>57</v>
+        <v>175</v>
       </c>
       <c r="W48">
-        <v>22.3</v>
+        <v>19</v>
       </c>
       <c r="X48">
-        <v>0.37</v>
+        <v>0.88</v>
       </c>
       <c r="Y48">
-        <v>0.37</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z48">
-        <v>0.13</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AA48">
-        <v>0.16</v>
+        <v>0.01</v>
       </c>
       <c r="AB48">
-        <v>2</v>
+        <v>24.6</v>
       </c>
       <c r="AC48">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="B49">
-        <v>26</v>
+        <v>180</v>
       </c>
       <c r="C49">
-        <v>0.1</v>
+        <v>16</v>
       </c>
       <c r="D49">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G49">
-        <v>426</v>
+        <v>1.2</v>
       </c>
       <c r="H49">
-        <v>0.05</v>
+        <v>0.44</v>
       </c>
       <c r="I49">
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J49">
-        <v>0.6</v>
+        <v>2.6</v>
       </c>
       <c r="K49">
-        <v>0.29799999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="L49">
-        <v>6.0999999999999999E-2</v>
+        <v>0.22</v>
       </c>
       <c r="N49">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="O49">
+        <v>0.42</v>
       </c>
       <c r="P49">
-        <v>9</v>
-      </c>
-      <c r="R49">
-        <v>1.06</v>
-      </c>
-      <c r="S49">
-        <v>1.1000000000000001</v>
+        <v>0.42</v>
       </c>
       <c r="T49">
-        <v>340</v>
+        <v>172</v>
       </c>
       <c r="U49">
-        <v>21</v>
+        <v>8.4</v>
       </c>
       <c r="V49">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="W49">
-        <v>12</v>
+        <v>11.4</v>
       </c>
       <c r="X49">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="Y49">
-        <v>0.32</v>
+        <v>1.32</v>
       </c>
       <c r="Z49">
-        <v>0.127</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AA49">
-        <v>0.125</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AB49">
-        <v>0.3</v>
+        <v>14.76</v>
       </c>
       <c r="AC49">
-        <v>1</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B50">
-        <v>359</v>
+        <v>72</v>
       </c>
       <c r="C50">
-        <v>1.3</v>
+        <v>0.26</v>
       </c>
       <c r="D50">
-        <v>79.8</v>
+        <v>16</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="F50">
-        <v>6.94</v>
+        <v>1.81</v>
       </c>
       <c r="H50">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="I50">
-        <v>1.2999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J50">
-        <v>1.48</v>
-      </c>
-      <c r="K50">
-        <v>0.39</v>
+        <v>1.58</v>
       </c>
       <c r="L50">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="N50">
-        <v>97</v>
-      </c>
-      <c r="R50">
-        <v>0.04</v>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="P50">
+        <v>23.3</v>
+      </c>
+      <c r="S50">
+        <v>0.8</v>
       </c>
       <c r="T50">
-        <v>35</v>
+        <v>446</v>
       </c>
       <c r="U50">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="V50">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="W50">
-        <v>12</v>
+        <v>22.3</v>
       </c>
       <c r="X50">
-        <v>1.2</v>
+        <v>0.37</v>
       </c>
       <c r="Y50">
-        <v>0.49</v>
+        <v>0.37</v>
       </c>
       <c r="Z50">
-        <v>6.9000000000000006E-2</v>
+        <v>0.13</v>
       </c>
       <c r="AA50">
-        <v>0.47199999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="AB50">
-        <v>7.5</v>
+        <v>2</v>
       </c>
       <c r="AC50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="B51">
-        <v>270</v>
+        <v>26</v>
       </c>
       <c r="C51">
-        <v>3.6</v>
+        <v>0.1</v>
       </c>
       <c r="D51">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E51">
-        <v>5.3</v>
+        <v>2.8</v>
       </c>
       <c r="F51">
-        <v>9.4</v>
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>426</v>
       </c>
       <c r="H51">
-        <v>0.50700000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="I51">
-        <v>0.24</v>
+        <v>0.11</v>
       </c>
       <c r="J51">
-        <v>4.76</v>
+        <v>0.6</v>
       </c>
       <c r="K51">
-        <v>0.54800000000000004</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="L51">
-        <v>9.1999999999999998E-2</v>
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N51">
+        <v>16</v>
+      </c>
+      <c r="P51">
+        <v>9</v>
+      </c>
+      <c r="R51">
+        <v>1.06</v>
+      </c>
+      <c r="S51">
+        <v>1.1000000000000001</v>
       </c>
       <c r="T51">
-        <v>117</v>
+        <v>340</v>
       </c>
       <c r="U51">
-        <v>211</v>
+        <v>21</v>
       </c>
       <c r="V51">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="W51">
-        <v>26.9</v>
+        <v>12</v>
       </c>
       <c r="X51">
-        <v>3.36</v>
+        <v>0.8</v>
       </c>
       <c r="Y51">
-        <v>0.88</v>
+        <v>0.32</v>
       </c>
       <c r="Z51">
-        <v>0.124</v>
+        <v>0.127</v>
       </c>
       <c r="AA51">
-        <v>0.63200000000000001</v>
+        <v>0.125</v>
       </c>
       <c r="AB51">
-        <v>23.2</v>
+        <v>0.3</v>
       </c>
       <c r="AC51">
-        <v>400</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="D52">
-        <v>77</v>
+        <v>79.8</v>
       </c>
       <c r="E52">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>7</v>
+        <v>6.94</v>
+      </c>
+      <c r="H52">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="I52">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J52">
+        <v>1.48</v>
+      </c>
+      <c r="K52">
+        <v>0.39</v>
+      </c>
+      <c r="L52">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N52">
+        <v>97</v>
+      </c>
+      <c r="R52">
+        <v>0.04</v>
       </c>
       <c r="T52">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="U52">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="V52">
+        <v>43</v>
+      </c>
+      <c r="W52">
+        <v>12</v>
       </c>
       <c r="X52">
-        <v>1.0900000000000001</v>
+        <v>1.2</v>
+      </c>
+      <c r="Y52">
+        <v>0.49</v>
+      </c>
+      <c r="Z52">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AA52">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="AB52">
+        <v>7.5</v>
       </c>
       <c r="AC52">
-        <v>106</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B53">
-        <v>36</v>
+        <v>270</v>
       </c>
       <c r="C53">
-        <v>0.22</v>
+        <v>3.6</v>
       </c>
       <c r="D53">
-        <v>7.96</v>
+        <v>49</v>
       </c>
       <c r="E53">
-        <v>4.8600000000000003</v>
+        <v>5.3</v>
       </c>
       <c r="F53">
-        <v>0.64</v>
-      </c>
-      <c r="M53">
-        <v>3.7</v>
-      </c>
-      <c r="P53">
-        <v>59.6</v>
+        <v>9.4</v>
+      </c>
+      <c r="H53">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="I53">
+        <v>0.24</v>
+      </c>
+      <c r="J53">
+        <v>4.76</v>
+      </c>
+      <c r="K53">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="L53">
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="T53">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="U53">
-        <v>17</v>
+        <v>211</v>
       </c>
       <c r="V53">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="W53">
-        <v>12.5</v>
+        <v>26.9</v>
       </c>
       <c r="X53">
-        <v>0.26</v>
+        <v>3.36</v>
       </c>
       <c r="Y53">
-        <v>0.11</v>
+        <v>0.88</v>
       </c>
       <c r="Z53">
-        <v>3.5000000000000003E-2</v>
+        <v>0.124</v>
       </c>
       <c r="AA53">
-        <v>0.36799999999999999</v>
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="AB53">
+        <v>23.2</v>
       </c>
       <c r="AC53">
-        <v>2</v>
+        <v>400</v>
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="C54">
-        <v>0.32</v>
+        <v>3</v>
       </c>
       <c r="D54">
-        <v>99.7</v>
+        <v>77</v>
       </c>
       <c r="E54">
-        <v>99.7</v>
+        <v>40</v>
       </c>
       <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="I54">
-        <v>1.9E-2</v>
+        <v>7</v>
       </c>
       <c r="T54">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="U54">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="X54">
-        <v>0.05</v>
-      </c>
-      <c r="Y54">
-        <v>0.01</v>
-      </c>
-      <c r="Z54">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AB54">
-        <v>0.6</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="AC54">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B55">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C55">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="D55">
-        <v>3.9</v>
+        <v>7.96</v>
       </c>
       <c r="E55">
-        <v>2.6</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="F55">
-        <v>0.9</v>
-      </c>
-      <c r="G55">
-        <v>42</v>
-      </c>
-      <c r="H55">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="I55">
-        <v>1.9E-2</v>
-      </c>
-      <c r="J55">
-        <v>0.59399999999999997</v>
-      </c>
-      <c r="K55">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="L55">
-        <v>0.08</v>
+        <v>0.64</v>
       </c>
       <c r="M55">
-        <v>0.7</v>
-      </c>
-      <c r="N55">
-        <v>15</v>
+        <v>3.7</v>
       </c>
       <c r="P55">
-        <v>13.7</v>
-      </c>
-      <c r="R55">
-        <v>0.54</v>
-      </c>
-      <c r="S55">
-        <v>7.9</v>
+        <v>59.6</v>
       </c>
       <c r="T55">
-        <v>237</v>
+        <v>161</v>
       </c>
       <c r="U55">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="V55">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W55">
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="X55">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="Y55">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
       <c r="Z55">
-        <v>5.8999999999999997E-2</v>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA55">
+        <v>0.36799999999999999</v>
       </c>
       <c r="AC55">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="B56">
-        <v>884</v>
+        <v>385</v>
       </c>
       <c r="C56">
-        <v>100</v>
+        <v>0.32</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>99.7</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>99.7</v>
       </c>
       <c r="F56">
         <v>0</v>
+      </c>
+      <c r="I56">
+        <v>1.9E-2</v>
+      </c>
+      <c r="T56">
+        <v>2</v>
+      </c>
+      <c r="U56">
+        <v>1</v>
+      </c>
+      <c r="X56">
+        <v>0.05</v>
+      </c>
+      <c r="Y56">
+        <v>0.01</v>
+      </c>
+      <c r="Z56">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AB56">
+        <v>0.6</v>
+      </c>
+      <c r="AC56">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="B57">
         <v>18</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>0.9</v>
+      </c>
+      <c r="G57">
+        <v>42</v>
+      </c>
+      <c r="H57">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I57">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J57">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="K57">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="L57">
+        <v>0.08</v>
+      </c>
+      <c r="M57">
+        <v>0.7</v>
+      </c>
+      <c r="N57">
+        <v>15</v>
+      </c>
+      <c r="P57">
+        <v>13.7</v>
+      </c>
+      <c r="R57">
+        <v>0.54</v>
+      </c>
+      <c r="S57">
+        <v>7.9</v>
+      </c>
+      <c r="T57">
+        <v>237</v>
+      </c>
+      <c r="U57">
+        <v>10</v>
+      </c>
+      <c r="V57">
+        <v>24</v>
+      </c>
+      <c r="W57">
+        <v>11</v>
+      </c>
+      <c r="X57">
+        <v>0.27</v>
+      </c>
+      <c r="Y57">
+        <v>0.17</v>
+      </c>
+      <c r="Z57">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AC57">
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B58">
-        <v>78</v>
+        <v>884</v>
       </c>
       <c r="C58">
-        <v>4.4800000000000004</v>
+        <v>100</v>
       </c>
       <c r="D58">
-        <v>5.57</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>4.09</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>3.82</v>
-      </c>
-      <c r="G58">
-        <v>48</v>
-      </c>
-      <c r="H58">
-        <v>5.5E-2</v>
-      </c>
-      <c r="I58">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="J58">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="L58">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="M58">
-        <v>3</v>
-      </c>
-      <c r="Q58">
-        <v>0.78</v>
-      </c>
-      <c r="S58">
-        <v>0.2</v>
-      </c>
-      <c r="T58">
-        <v>164</v>
-      </c>
-      <c r="U58">
-        <v>127</v>
-      </c>
-      <c r="V58">
-        <v>101</v>
-      </c>
-      <c r="W58">
-        <v>11.4</v>
-      </c>
-      <c r="X58">
-        <v>0.05</v>
-      </c>
-      <c r="Y58">
-        <v>0.43</v>
-      </c>
-      <c r="Z58">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AA58">
-        <v>2E-3</v>
-      </c>
-      <c r="AC58">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59">
+        <v>18</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60">
+        <v>78</v>
+      </c>
+      <c r="C60">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="D60">
+        <v>5.57</v>
+      </c>
+      <c r="E60">
+        <v>4.09</v>
+      </c>
+      <c r="F60">
+        <v>3.82</v>
+      </c>
+      <c r="G60">
+        <v>48</v>
+      </c>
+      <c r="H60">
+        <v>5.5E-2</v>
+      </c>
+      <c r="I60">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="J60">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L60">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M60">
+        <v>3</v>
+      </c>
+      <c r="Q60">
+        <v>0.78</v>
+      </c>
+      <c r="S60">
+        <v>0.2</v>
+      </c>
+      <c r="T60">
+        <v>164</v>
+      </c>
+      <c r="U60">
+        <v>127</v>
+      </c>
+      <c r="V60">
+        <v>101</v>
+      </c>
+      <c r="W60">
+        <v>11.4</v>
+      </c>
+      <c r="X60">
+        <v>0.05</v>
+      </c>
+      <c r="Y60">
+        <v>0.43</v>
+      </c>
+      <c r="Z60">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AA60">
+        <v>2E-3</v>
+      </c>
+      <c r="AC60">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B59">
+      <c r="B61">
         <v>19.8</v>
       </c>
-      <c r="C59">
+      <c r="C61">
         <v>0.22</v>
       </c>
-      <c r="D59">
+      <c r="D61">
         <v>4.1500000000000004</v>
       </c>
-      <c r="E59">
+      <c r="E61">
         <v>2.15</v>
       </c>
-      <c r="F59">
+      <c r="F61">
         <v>1.5</v>
       </c>
     </row>
@@ -3594,7 +3655,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G59 H47:AC47">
+  <conditionalFormatting sqref="G4:G61 H49:AC49">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -3606,7 +3667,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G60:G1048576 G1:G54 H55:H59 H47:AC47">
+  <conditionalFormatting sqref="G62:G1048576 G1:G56 H57:H61 H49:AC49">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -3618,7 +3679,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H60:H1048576 H1:H46 I55:I59 H48:H54">
+  <conditionalFormatting sqref="H62:H1048576 H1:H48 I57:I61 H50:H56">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -3630,7 +3691,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I60:I1048576 I1:I46 J55:J59 I48:I54">
+  <conditionalFormatting sqref="I62:I1048576 I1:I48 J57:J61 I50:I56">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -3642,7 +3703,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J60:J1048576 J1:J46 J48:J54">
+  <conditionalFormatting sqref="J62:J1048576 J1:J48 J50:J56">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -3654,7 +3715,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K48:K1048576 K1:K46">
+  <conditionalFormatting sqref="K50:K1048576 K1:K48">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -3666,7 +3727,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L48:L1048576 L1:L46">
+  <conditionalFormatting sqref="L50:L1048576 L1:L48">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -3678,7 +3739,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M48:M1048576 M1:M46">
+  <conditionalFormatting sqref="M50:M1048576 M1:M48">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -3690,7 +3751,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N48:N1048576 N1:N46">
+  <conditionalFormatting sqref="N50:N1048576 N1:N48">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -3702,7 +3763,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O48:O1048576 O1:O46">
+  <conditionalFormatting sqref="O50:O1048576 O1:O48">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3714,7 +3775,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P48:P1048576 P1:P46">
+  <conditionalFormatting sqref="P50:P1048576 P1:P48">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -3726,7 +3787,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q48:Q1048576 Q1:Q46">
+  <conditionalFormatting sqref="Q50:Q1048576 Q1:Q48">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3738,7 +3799,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R48:R1048576 R1:R46">
+  <conditionalFormatting sqref="R50:R1048576 R1:R48">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -3750,7 +3811,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S48:S1048576 S1:S46">
+  <conditionalFormatting sqref="S50:S1048576 S1:S48">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3762,7 +3823,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T48:T1048576 T1:T46">
+  <conditionalFormatting sqref="T50:T1048576 T1:T48">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -3774,7 +3835,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U48:U1048576 U1:U46">
+  <conditionalFormatting sqref="U50:U1048576 U1:U48">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -3786,7 +3847,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V48:V1048576 V1:V46">
+  <conditionalFormatting sqref="V50:V1048576 V1:V48">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3798,7 +3859,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W48:W1048576 W1:W46">
+  <conditionalFormatting sqref="W50:W1048576 W1:W48">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -3810,7 +3871,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X48:X1048576 X1:X46">
+  <conditionalFormatting sqref="X50:X1048576 X1:X48">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -3822,7 +3883,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y48:Y1048576 Y1:Y46">
+  <conditionalFormatting sqref="Y50:Y1048576 Y1:Y48">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3834,7 +3895,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z48:Z1048576 Z1:Z46">
+  <conditionalFormatting sqref="Z50:Z1048576 Z1:Z48">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3846,7 +3907,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA48:AA1048576 AA1:AA46">
+  <conditionalFormatting sqref="AA50:AA1048576 AA1:AA48">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3858,7 +3919,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB48:AB1048576 AB1:AB46">
+  <conditionalFormatting sqref="AB50:AB1048576 AB1:AB48">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3870,7 +3931,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC48:AC1048576 AC1:AC46">
+  <conditionalFormatting sqref="AC50:AC1048576 AC1:AC48">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>